<commit_message>
upload lastest version to github
</commit_message>
<xml_diff>
--- a/raw_data/model/model_summary.xlsx
+++ b/raw_data/model/model_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dennischeng\code\dennischengsc\safety_detection\raw_data\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81284F45-FD6F-4EFB-ABFC-89C8259852E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9588CE63-F5FF-406F-931F-110D4ED04DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" xr2:uid="{6026F88D-6E7A-4362-AC3C-5B80CD364329}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Dennis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -132,6 +132,10 @@
   </si>
   <si>
     <t>mAP50-95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adam</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -140,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0000_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -330,7 +334,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -355,22 +359,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,20 +412,26 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-SG" altLang="zh-TW"/>
+              <a:rPr lang="en-SG"/>
               <a:t>Yolov8 Model Comparision</a:t>
             </a:r>
           </a:p>
@@ -443,13 +450,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -480,13 +493,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -554,13 +573,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -591,6 +616,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.36542027976752001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26333017178296297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24420591810470299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.5445944150040193E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -616,13 +653,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -690,13 +733,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -746,6 +795,86 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6591-4751-8334-7F53BA5ED2D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adam</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mAP50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mAP50-95</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$6:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.87629754558529904</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66717248475942803</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74941635595471801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46033438142011701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F734-41F6-A980-78340829596C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -776,9 +905,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -792,9 +921,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -823,9 +951,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -851,9 +979,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -868,6 +995,43 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -893,9 +1057,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -919,17 +1082,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -992,35 +1166,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1028,26 +1200,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1056,9 +1236,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1077,14 +1256,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1093,45 +1264,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1143,31 +1304,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1185,21 +1344,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1209,20 +1365,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1236,14 +1392,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1257,9 +1413,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1273,12 +1428,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1290,9 +1439,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1307,108 +1456,115 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1420,12 +1576,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1441,7 +1604,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1450,9 +1612,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1462,7 +1623,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1470,9 +1631,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1483,9 +1644,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1497,12 +1657,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1511,16 +1665,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>298939</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>111369</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>334110</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>67406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>43962</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>99646</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>88561</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57595</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1847,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC07325C-D83E-4A51-AC50-0684E5D8988E}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1898,16 +2052,16 @@
       <c r="J1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1942,16 +2096,16 @@
       <c r="J2" s="4">
         <v>0.01</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>0.90256892959999802</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>0.73491803577205395</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <v>0.80803145585539105</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <v>0.516648408962598</v>
       </c>
     </row>
@@ -1986,10 +2140,18 @@
       <c r="J3" s="4">
         <v>0.01</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="11"/>
+      <c r="K3" s="9">
+        <v>0.36542027976752001</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.26333017178296297</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.24420591810470299</v>
+      </c>
+      <c r="N3" s="10">
+        <v>9.5445944150040193E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
@@ -2022,16 +2184,16 @@
       <c r="J4" s="4">
         <v>0.01</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>0.89677804470649303</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>0.71047171267188902</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>0.784690155515268</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>0.48423904652962801</v>
       </c>
     </row>
@@ -2066,23 +2228,78 @@
       <c r="J5" s="6">
         <v>0.01</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>0.90180730968628497</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>0.76099995227395201</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11">
         <v>0.82900442135933905</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="12">
         <v>0.54402590460381905</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="6" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>640</v>
+      </c>
+      <c r="C6" s="4">
+        <v>200</v>
+      </c>
+      <c r="D6" s="4">
+        <v>32</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.87629754558529904</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.66717248475942803</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0.74941635595471801</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0.46033438142011701</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:J5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:J6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
udpate app.py and herlp.py
</commit_message>
<xml_diff>
--- a/raw_data/model/model_summary.xlsx
+++ b/raw_data/model/model_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dennischeng\code\dennischengsc\safety_detection\raw_data\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37AC381-0585-4517-889A-C26CCD754AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6250A484-70D8-4C98-A23F-82C9B6904D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" activeTab="1" xr2:uid="{6026F88D-6E7A-4362-AC3C-5B80CD364329}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>Dennis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lr = 0.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>learning rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,12 +194,18 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -355,7 +357,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -393,6 +395,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1296,6 +1304,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.89029697707704303</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72881881085403999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80682552827054899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50599967990122696</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1315,7 +1335,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lr = 0.005</c:v>
+                  <c:v>lr = 0.05</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1364,6 +1384,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.90525550000421295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71998515088187098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80524557074299996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52664764717956503</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1432,6 +1464,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.90617152563783598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73815589679274096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79631229045646301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50680627417865498</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1451,7 +1495,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lr = 0.1</c:v>
+                  <c:v>lr = 0.005</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1500,6 +1544,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.92048765589733295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75935411970159195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83718223381212797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55267262599724098</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3493,7 +3549,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3541,7 +3597,7 @@
         <v>12</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>22</v>
@@ -3587,10 +3643,18 @@
       <c r="J2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="10"/>
+      <c r="K2" s="9">
+        <v>0.89029697707704303</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.72881881085403999</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0.80682552827054899</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0.50599967990122696</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
@@ -3621,12 +3685,20 @@
         <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.90525550000421295</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.71998515088187098</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.80524557074299996</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0.52664764717956503</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
@@ -3659,10 +3731,18 @@
       <c r="J4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
+      <c r="K4" s="9">
+        <v>0.90617152563783598</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.73815589679274096</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.79631229045646301</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0.50680627417865498</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="5" t="s">
@@ -3693,12 +3773,20 @@
         <v>16</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0.92048765589733295</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0.75935411970159195</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0.83718223381212797</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0.55267262599724098</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>

</xml_diff>

<commit_message>
all master files tally
</commit_message>
<xml_diff>
--- a/raw_data/model/model_summary.xlsx
+++ b/raw_data/model/model_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dennischeng\code\dennischengsc\safety_detection\raw_data\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37AC381-0585-4517-889A-C26CCD754AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6250A484-70D8-4C98-A23F-82C9B6904D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" activeTab="1" xr2:uid="{6026F88D-6E7A-4362-AC3C-5B80CD364329}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>Dennis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lr = 0.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>learning rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,12 +194,18 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -355,7 +357,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -393,6 +395,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1296,6 +1304,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.89029697707704303</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72881881085403999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80682552827054899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50599967990122696</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1315,7 +1335,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lr = 0.005</c:v>
+                  <c:v>lr = 0.05</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1364,6 +1384,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.90525550000421295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71998515088187098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80524557074299996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52664764717956503</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1432,6 +1464,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.90617152563783598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73815589679274096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79631229045646301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50680627417865498</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1451,7 +1495,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lr = 0.1</c:v>
+                  <c:v>lr = 0.005</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1500,6 +1544,18 @@
               <c:numCache>
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.92048765589733295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75935411970159195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83718223381212797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55267262599724098</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3493,7 +3549,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3541,7 +3597,7 @@
         <v>12</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>22</v>
@@ -3587,10 +3643,18 @@
       <c r="J2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="10"/>
+      <c r="K2" s="9">
+        <v>0.89029697707704303</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.72881881085403999</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0.80682552827054899</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0.50599967990122696</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
@@ -3621,12 +3685,20 @@
         <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.90525550000421295</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.71998515088187098</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.80524557074299996</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0.52664764717956503</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
@@ -3659,10 +3731,18 @@
       <c r="J4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
+      <c r="K4" s="9">
+        <v>0.90617152563783598</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.73815589679274096</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.79631229045646301</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0.50680627417865498</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="5" t="s">
@@ -3693,12 +3773,20 @@
         <v>16</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0.92048765589733295</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0.75935411970159195</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0.83718223381212797</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0.55267262599724098</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>

</xml_diff>